<commit_message>
Replaced all instances of the term squad with the term unit; likewise with the terms unit and model. This reflects the language used in the actual 40k ruleset.
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B697CF-CC5D-415B-B372-E077340D8B43}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FB4E9E-4884-4660-9FEB-05AEE3FF5A62}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="1" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="2" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Templar Ranged Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Templar Melee Weapons" sheetId="4" r:id="rId2"/>
-    <sheet name="Templar Units" sheetId="2" r:id="rId3"/>
+    <sheet name="Templar Models" sheetId="2" r:id="rId3"/>
     <sheet name="Army Sheet" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1349,7 +1349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9B6098-EF80-434F-8A4C-B8A7BE87648E}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
@@ -1492,9 +1492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC9FF83-A4B4-495A-8CD6-852B5A72C621}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Integrated model stats from text-based sim
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FB4E9E-4884-4660-9FEB-05AEE3FF5A62}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E62257-E759-43C2-AD08-32F210DAA92D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="2" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Weapon</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Attacks function</t>
+  </si>
+  <si>
+    <t>Radius</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -295,11 +298,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -334,6 +348,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,7 +1509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,6 +1590,9 @@
       <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L2" s="16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1607,6 +1625,9 @@
       <c r="J3">
         <v>3</v>
       </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1639,6 +1660,9 @@
       <c r="J4">
         <v>4</v>
       </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1671,6 +1695,9 @@
       <c r="J5">
         <v>3</v>
       </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1703,6 +1730,9 @@
       <c r="J8">
         <v>6</v>
       </c>
+      <c r="L8">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1735,6 +1765,9 @@
       <c r="J9">
         <v>6</v>
       </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1766,6 +1799,9 @@
       </c>
       <c r="J10">
         <v>6</v>
+      </c>
+      <c r="L10">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Plague Marine targets to Orks; Plague Marines were much too hard to kill.
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E62257-E759-43C2-AD08-32F210DAA92D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71967C7-262F-4A33-A6D0-0FEB4C98195B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="2" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
@@ -1509,7 +1509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented morale losses. Added more models to each unit better test morale. Added some test friendly weapons and models for future testing purposes. Added brackets to unit names to improve readability of console debug text.
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\git\40k\pygame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Git\40k-Pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01311684-421D-44EA-ABCF-294CF2F6B71A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A458995-FB08-4DC1-AC41-B14AB8D3B599}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6465" activeTab="1" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
+    <workbookView xWindow="28680" yWindow="990" windowWidth="21840" windowHeight="13740" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Templar Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,23 @@
     <sheet name="Templar Models" sheetId="2" r:id="rId3"/>
     <sheet name="Army Sheet" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Weapon</t>
   </si>
@@ -247,6 +253,12 @@
   </si>
   <si>
     <t>CCW</t>
+  </si>
+  <si>
+    <t>Test Ork</t>
+  </si>
+  <si>
+    <t>Test Gun</t>
   </si>
 </sst>
 </file>
@@ -683,9 +695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDAFB37-BC4F-43E6-8574-A43CDCD4006E}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6">
         <v>4</v>
@@ -1065,6 +1077,35 @@
       </c>
       <c r="L11" s="11" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>5</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1382,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9B6098-EF80-434F-8A4C-B8A7BE87648E}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
@@ -1577,7 +1618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,6 +1805,41 @@
         <v>3</v>
       </c>
       <c r="L5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="L7">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted test gun stats, gave it to all models to better test wound allocation and morale. Moved more orks to the back of the map to make ray tracing step go faster during testing. Fixed error message spam during wound allocation.
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Git\40k-Pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A458995-FB08-4DC1-AC41-B14AB8D3B599}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050F16BF-4EFA-4634-9230-9FDB9D0E7BFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="990" windowWidth="21840" windowHeight="13740" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>Weapon</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>Poweraxe</t>
-  </si>
-  <si>
-    <t>Powerfist</t>
   </si>
   <si>
     <t>User</t>
@@ -697,7 +694,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="5">
         <v>12</v>
@@ -1425,7 +1422,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,27 +1486,27 @@
         <v>4</v>
       </c>
       <c r="F2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1529,7 +1526,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
@@ -1549,7 +1546,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="8">
         <v>-3</v>
@@ -1582,9 +1579,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="A7" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
@@ -1700,7 +1695,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1810,7 +1805,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -1950,7 +1945,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -1985,7 +1980,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14">
         <v>5</v>

</xml_diff>

<commit_message>
Debugged morale phase. Brought Test Gun values down a bit (it was wounding too often)
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Git\40k-Pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050F16BF-4EFA-4634-9230-9FDB9D0E7BFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA5B351-FC48-4C50-B21A-09C820F75955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="990" windowWidth="21840" windowHeight="13740" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="6">
         <v>2</v>
@@ -1613,7 +1613,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented a dreadnought into the game to test the game's ability to handle both large models as well as single model units. Ended up discovering several bugs: inverse ap for melee weapons, multi-damage attacks are split into single wounds packets.
</commit_message>
<xml_diff>
--- a/40k_sim_workbook.xlsx
+++ b/40k_sim_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Git\40k-Pygame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA5B351-FC48-4C50-B21A-09C820F75955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9B0C37-351D-420E-BA10-DB6C4DD60A95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="990" windowWidth="21840" windowHeight="13740" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
+    <workbookView xWindow="12510" yWindow="855" windowWidth="15210" windowHeight="10335" activeTab="1" xr2:uid="{25CACC89-7CFE-40F5-86BB-4DBD087764E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Templar Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>Weapon</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>Test Gun</t>
+  </si>
+  <si>
+    <t>Assault Cannon</t>
+  </si>
+  <si>
+    <t>Dreadnought</t>
+  </si>
+  <si>
+    <t>Dreadnought Combat Weapon</t>
+  </si>
+  <si>
+    <t>2x</t>
   </si>
 </sst>
 </file>
@@ -690,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDAFB37-BC4F-43E6-8574-A43CDCD4006E}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,6 +1422,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="5">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>6</v>
+      </c>
+      <c r="F30" s="5">
+        <v>6</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1420,9 +1461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9B6098-EF80-434F-8A4C-B8A7BE87648E}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1590,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="8">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -1569,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D6" s="8">
         <v>0</v>
@@ -1580,6 +1621,23 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
@@ -1609,11 +1667,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC9FF83-A4B4-495A-8CD6-852B5A72C621}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,6 +2069,41 @@
       </c>
       <c r="L14">
         <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>